<commit_message>
Updated process data code
</commit_message>
<xml_diff>
--- a/DataProcessing/results_exp2.xlsx
+++ b/DataProcessing/results_exp2.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvirbenasuli13/Documents/GitHub/ShapeFromMotionV4/DataProcessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE280B4-611E-0C43-8911-C66274B48D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E23AA34-8D64-0E4D-88EC-F7000C8A9C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18040" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34160" yWindow="460" windowWidth="18040" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mean" sheetId="1" r:id="rId1"/>
     <sheet name="STD" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Mean A</t>
   </si>
@@ -48,12 +48,15 @@
   <si>
     <t>Mean</t>
   </si>
+  <si>
+    <t>std</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -63,12 +66,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -93,11 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E973"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62:D81"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62:E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,1147 +431,1385 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>8</v>
       </c>
       <c r="C2">
         <v>0.1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.8</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>11</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>17</v>
       </c>
       <c r="C3">
         <v>0.1</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="1"/>
+      <c r="D3" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>11</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4">
         <v>0.1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>13</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>8</v>
       </c>
       <c r="C5">
         <v>0.1</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>14</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>8</v>
       </c>
       <c r="C6">
         <v>0.1</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>17</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>7</v>
       </c>
       <c r="C7">
         <v>0.1</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.85</v>
+      <c r="D7" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.13</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>17</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>11</v>
       </c>
       <c r="C8">
         <v>0.1</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.95</v>
+      <c r="D8" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.09</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>3</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>11</v>
       </c>
       <c r="C9">
         <v>0.1</v>
       </c>
-      <c r="D9" s="3">
-        <v>0.25</v>
+      <c r="D9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>3</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>7</v>
       </c>
       <c r="C10">
         <v>0.1</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.35</v>
+      <c r="D10" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>6</v>
       </c>
       <c r="C11">
         <v>0.1</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.5</v>
+      <c r="D11" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.33</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>6</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>5</v>
       </c>
       <c r="C12">
         <v>0.1</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.8</v>
+      <c r="D12" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>6.5</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>11</v>
       </c>
       <c r="C13">
         <v>0.1</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.1</v>
+      <c r="D13" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.21</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>7</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>17</v>
       </c>
       <c r="C14">
         <v>0.1</v>
       </c>
-      <c r="D14" s="2">
-        <v>0.1</v>
+      <c r="D14" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.21</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>7</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>3</v>
       </c>
       <c r="C15">
         <v>0.1</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
+      <c r="E15" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>8</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>10</v>
       </c>
       <c r="C16">
         <v>0.1</v>
       </c>
-      <c r="D16" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="D16" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>8</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>12</v>
       </c>
       <c r="C17">
         <v>0.1</v>
       </c>
-      <c r="D17" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="D17" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>8</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>13</v>
       </c>
       <c r="C18">
         <v>0.1</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="E18" s="1">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>8</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>14</v>
       </c>
       <c r="C19">
         <v>0.1</v>
       </c>
-      <c r="D19" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="D19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>8</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>6</v>
       </c>
       <c r="C20">
         <v>0.1</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="E20" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>9</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>18</v>
       </c>
       <c r="C21">
         <v>0.1</v>
       </c>
-      <c r="D21" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="D21" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>10</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>8</v>
       </c>
       <c r="C22">
         <v>0.4</v>
       </c>
-      <c r="D22" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="D22" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>11</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>17</v>
       </c>
       <c r="C23">
         <v>0.4</v>
       </c>
-      <c r="D23" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="D23" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>11</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>3</v>
       </c>
       <c r="C24">
         <v>0.4</v>
       </c>
-      <c r="D24" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="D24" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>13</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>8</v>
       </c>
       <c r="C25">
         <v>0.4</v>
       </c>
-      <c r="D25" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="D25" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>14</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>8</v>
       </c>
       <c r="C26">
         <v>0.4</v>
       </c>
-      <c r="D26" s="2">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="D26" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>17</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>7</v>
       </c>
       <c r="C27">
         <v>0.4</v>
       </c>
-      <c r="D27" s="2">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="D27" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>17</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>11</v>
       </c>
       <c r="C28">
         <v>0.4</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="E28" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>3</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>11</v>
       </c>
       <c r="C29">
         <v>0.4</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="E29" s="1">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>3</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>7</v>
       </c>
       <c r="C30">
         <v>0.4</v>
       </c>
-      <c r="D30" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="D30" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>5</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>6</v>
       </c>
       <c r="C31">
         <v>0.4</v>
       </c>
-      <c r="D31" s="2">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="D31" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>6</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>5</v>
       </c>
       <c r="C32">
         <v>0.4</v>
       </c>
-      <c r="D32" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="D32" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>6.5</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>11</v>
       </c>
       <c r="C33">
         <v>0.4</v>
       </c>
-      <c r="D33" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="D33" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>7</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>17</v>
       </c>
       <c r="C34">
         <v>0.4</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="E34" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
         <v>7</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>3</v>
       </c>
       <c r="C35">
         <v>0.4</v>
       </c>
-      <c r="D35" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+      <c r="D35" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
         <v>8</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>10</v>
       </c>
       <c r="C36">
         <v>0.4</v>
       </c>
-      <c r="D36" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+      <c r="D36" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
         <v>8</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>12</v>
       </c>
       <c r="C37">
         <v>0.4</v>
       </c>
-      <c r="D37" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="D37" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
         <v>8</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>13</v>
       </c>
       <c r="C38">
         <v>0.4</v>
       </c>
-      <c r="D38" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+      <c r="D38" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <v>8</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>14</v>
       </c>
       <c r="C39">
         <v>0.4</v>
       </c>
-      <c r="D39" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+      <c r="D39" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
         <v>8</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>6</v>
       </c>
       <c r="C40">
         <v>0.4</v>
       </c>
-      <c r="D40" s="2">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+      <c r="D40" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
         <v>9</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>18</v>
       </c>
       <c r="C41">
         <v>0.4</v>
       </c>
-      <c r="D41" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+      <c r="D41" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>10</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>8</v>
       </c>
       <c r="C42">
         <v>0.7</v>
       </c>
-      <c r="D42" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
+      <c r="D42" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
         <v>11</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>17</v>
       </c>
       <c r="C43">
         <v>0.7</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E43" s="1">
         <v>0.25</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>11</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>3</v>
       </c>
       <c r="C44">
         <v>0.7</v>
       </c>
-      <c r="D44" s="2">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
+      <c r="D44" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>13</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>8</v>
       </c>
       <c r="C45">
         <v>0.7</v>
       </c>
-      <c r="D45" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
+      <c r="D45" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>14</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>8</v>
       </c>
       <c r="C46">
         <v>0.7</v>
       </c>
-      <c r="D46" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
+      <c r="D46" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>17</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>7</v>
       </c>
       <c r="C47">
         <v>0.7</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+      <c r="E47" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>17</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>11</v>
       </c>
       <c r="C48">
         <v>0.7</v>
       </c>
-      <c r="D48" s="2">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
+      <c r="D48" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>3</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>11</v>
       </c>
       <c r="C49">
         <v>0.7</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="E49" s="1">
         <v>0.35</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>3</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>7</v>
       </c>
       <c r="C50">
         <v>0.7</v>
       </c>
-      <c r="D50" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
+      <c r="D50" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>5</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>6</v>
       </c>
       <c r="C51">
         <v>0.7</v>
       </c>
-      <c r="D51" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
+      <c r="D51" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
         <v>6</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>5</v>
       </c>
       <c r="C52">
         <v>0.7</v>
       </c>
-      <c r="D52" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
+      <c r="D52" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>6.5</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>11</v>
       </c>
       <c r="C53">
         <v>0.7</v>
       </c>
-      <c r="D53" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
+      <c r="D53" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
         <v>7</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>17</v>
       </c>
       <c r="C54">
         <v>0.7</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2">
+      <c r="E54" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
         <v>7</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>3</v>
       </c>
       <c r="C55">
         <v>0.7</v>
       </c>
-      <c r="D55" s="2">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="2">
+      <c r="D55" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
         <v>8</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>10</v>
       </c>
       <c r="C56">
         <v>0.7</v>
       </c>
-      <c r="D56" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="2">
+      <c r="D56" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
         <v>8</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>12</v>
       </c>
       <c r="C57">
         <v>0.7</v>
       </c>
-      <c r="D57" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="2">
+      <c r="D57" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>8</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>13</v>
       </c>
       <c r="C58">
         <v>0.7</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
+      <c r="E58" s="1">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
         <v>8</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>14</v>
       </c>
       <c r="C59">
         <v>0.7</v>
       </c>
-      <c r="D59" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
+      <c r="D59" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
         <v>8</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>6</v>
       </c>
       <c r="C60">
         <v>0.7</v>
       </c>
-      <c r="D60" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="2">
+      <c r="D60" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>9</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>18</v>
       </c>
       <c r="C61">
         <v>0.7</v>
       </c>
-      <c r="D61" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="2">
+      <c r="D61" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
         <v>10</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>8</v>
       </c>
       <c r="C62">
         <v>1.5</v>
       </c>
-      <c r="D62" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
+      <c r="D62" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
         <v>11</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>17</v>
       </c>
       <c r="C63">
         <v>1.5</v>
       </c>
-      <c r="D63" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
+      <c r="D63" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
         <v>11</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>3</v>
       </c>
       <c r="C64">
         <v>1.5</v>
       </c>
-      <c r="D64" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2">
+      <c r="D64" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
         <v>13</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="1">
         <v>8</v>
       </c>
       <c r="C65">
         <v>1.5</v>
       </c>
-      <c r="D65" s="2">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2">
+      <c r="D65" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
         <v>14</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>8</v>
       </c>
       <c r="C66">
         <v>1.5</v>
       </c>
-      <c r="D66" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2">
+      <c r="D66" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
         <v>17</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>7</v>
       </c>
       <c r="C67">
         <v>1.5</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="2">
+      <c r="E67" s="1">
+        <v>7.4535599250000001E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>17</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>11</v>
       </c>
       <c r="C68">
         <v>1.5</v>
       </c>
-      <c r="D68" s="2">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="2">
+      <c r="D68" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
         <v>3</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>11</v>
       </c>
       <c r="C69">
         <v>1.5</v>
       </c>
-      <c r="D69" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="2">
+      <c r="D69" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
         <v>3</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>7</v>
       </c>
       <c r="C70">
         <v>1.5</v>
       </c>
-      <c r="D70" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="2">
+      <c r="D70" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>5</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>6</v>
       </c>
       <c r="C71">
         <v>1.5</v>
       </c>
-      <c r="D71" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="2">
+      <c r="D71" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
         <v>6</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>5</v>
       </c>
       <c r="C72">
         <v>1.5</v>
       </c>
-      <c r="D72" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="2">
+      <c r="D72" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
         <v>6.5</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>11</v>
       </c>
       <c r="C73">
         <v>1.5</v>
       </c>
-      <c r="D73" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="2">
+      <c r="D73" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
         <v>7</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="1">
         <v>17</v>
       </c>
       <c r="C74">
         <v>1.5</v>
       </c>
-      <c r="D74" s="2">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="2">
+      <c r="D74" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
         <v>7</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>3</v>
       </c>
       <c r="C75">
         <v>1.5</v>
       </c>
-      <c r="D75" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="2">
+      <c r="D75" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
         <v>8</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>10</v>
       </c>
       <c r="C76">
         <v>1.5</v>
       </c>
-      <c r="D76" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="2">
+      <c r="D76" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
         <v>8</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="1">
         <v>12</v>
       </c>
       <c r="C77">
         <v>1.5</v>
       </c>
-      <c r="D77" s="2">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="2">
+      <c r="D77" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
         <v>8</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>13</v>
       </c>
       <c r="C78">
         <v>1.5</v>
       </c>
-      <c r="D78" s="2">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="2">
+      <c r="D78" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
         <v>8</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>14</v>
       </c>
       <c r="C79">
         <v>1.5</v>
       </c>
-      <c r="D79" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="2">
+      <c r="D79" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
         <v>8</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>6</v>
       </c>
       <c r="C80">
         <v>1.5</v>
       </c>
-      <c r="D80" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="2">
+      <c r="D80" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
         <v>9</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="1">
         <v>18</v>
       </c>
       <c r="C81">
         <v>1.5</v>
       </c>
-      <c r="D81" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D81" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2462,10 +2695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D979"/>
+  <dimension ref="A1:E979"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44:D64"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2475,7 +2708,7 @@
     <col min="5" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2488,887 +2721,1079 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1.5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0.1</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="E2" s="1">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.7</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="E3" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>0.3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.9</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="E4" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>1.3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.3</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="E5" s="1">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>2.5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="E6" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>0.1</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="E7" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>0.1</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>1.5</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="D8" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>0.7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="D9" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>0.9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0.3</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="D10" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>0.3</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>1.3</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="D11" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>2.5</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="D12" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>0.1</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="D13" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>1.5</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14">
         <v>5</v>
       </c>
-      <c r="D14" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="D14" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>1.5</v>
       </c>
       <c r="C15">
         <v>5</v>
       </c>
-      <c r="D15" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="D15" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>2</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
-      <c r="D16" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="D16" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>2</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
-      <c r="D17" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="D17" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>0.5</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>1.5</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
-      <c r="D18" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="D18" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>2.5</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>2.25</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
-      <c r="D19" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="D19" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>2.25</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>1.25</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
-      <c r="D20" s="2">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="D20" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>2.25</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>1.75</v>
       </c>
       <c r="C21">
         <v>5</v>
       </c>
-      <c r="D21" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="D21" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>1.5</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>0.5</v>
       </c>
       <c r="C22">
         <v>5</v>
       </c>
-      <c r="D22" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="D22" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>1.5</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>0.1</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="E23" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>2</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>0.7</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="E24" s="1">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>0.3</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>0.9</v>
       </c>
       <c r="C25">
         <v>10</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="E25" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>1.3</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>0.3</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="E26" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>2.5</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>1</v>
       </c>
       <c r="C27">
         <v>10</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="E27" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>0.1</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>1</v>
       </c>
       <c r="C28">
         <v>10</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="E28" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>0.1</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>1.5</v>
       </c>
       <c r="C29">
         <v>10</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="E29" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>0.7</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>2</v>
       </c>
       <c r="C30">
         <v>10</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="E30" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>0.9</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>0.3</v>
       </c>
       <c r="C31">
         <v>10</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="E31" s="1">
         <v>0.3</v>
       </c>
-      <c r="B32" s="2">
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B32" s="1">
         <v>1.3</v>
       </c>
       <c r="C32">
         <v>10</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="E32" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>1</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>2.5</v>
       </c>
       <c r="C33">
         <v>10</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="E33" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>1</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>0.1</v>
       </c>
       <c r="C34">
         <v>10</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="E34" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
         <v>1.5</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>1</v>
       </c>
       <c r="C35">
         <v>10</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+      <c r="E35" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
         <v>1</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>1.5</v>
       </c>
       <c r="C36">
         <v>10</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+      <c r="E36" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
         <v>2</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>1</v>
       </c>
       <c r="C37">
         <v>10</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="1">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="E37" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
         <v>1</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>2</v>
       </c>
       <c r="C38">
         <v>10</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+      <c r="E38" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <v>0.5</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>1.5</v>
       </c>
       <c r="C39">
         <v>10</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+      <c r="E39" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
         <v>2.5</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>2.25</v>
       </c>
       <c r="C40">
         <v>10</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+      <c r="E40" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
         <v>2.25</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>1.25</v>
       </c>
       <c r="C41">
         <v>10</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+      <c r="E41" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>2.25</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>1.75</v>
       </c>
       <c r="C42">
         <v>10</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
+      <c r="E42" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
         <v>1.5</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>0.5</v>
       </c>
       <c r="C43">
         <v>10</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+      <c r="E43" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>1.5</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>0.1</v>
       </c>
       <c r="C44">
         <v>15</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="1">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
+      <c r="E44" s="1">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>2</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>0.7</v>
       </c>
       <c r="C45">
         <v>15</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="1">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
+      <c r="E45" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>0.3</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>0.9</v>
       </c>
       <c r="C46">
         <v>15</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="1">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
+      <c r="E46" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>1.3</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>0.3</v>
       </c>
       <c r="C47">
         <v>15</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="1">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+      <c r="E47" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>2.5</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>1</v>
       </c>
       <c r="C48">
         <v>15</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="1">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
+      <c r="E48" s="1">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>0.1</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>1</v>
       </c>
       <c r="C49">
         <v>15</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="1">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+      <c r="E49" s="1">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>0.1</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>1.5</v>
       </c>
       <c r="C50">
         <v>15</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="1">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
+      <c r="E50" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>0.7</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>2</v>
       </c>
       <c r="C51">
         <v>15</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
+      <c r="E51" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
         <v>0.9</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>0.3</v>
       </c>
       <c r="C52">
         <v>15</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
+      <c r="E52" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>0.3</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>1.3</v>
       </c>
       <c r="C53">
         <v>15</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="1">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
+      <c r="E53" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
         <v>1</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>2.5</v>
       </c>
       <c r="C54">
         <v>15</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2">
+      <c r="E54" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
         <v>1</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>0.1</v>
       </c>
       <c r="C55">
         <v>15</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="2">
+      <c r="E55" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
         <v>1.5</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>1</v>
       </c>
       <c r="C56">
         <v>15</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="2">
+      <c r="E56" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
         <v>1</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>1.5</v>
       </c>
       <c r="C57">
         <v>15</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="2">
+      <c r="E57" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>2</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>1</v>
       </c>
       <c r="C58">
         <v>15</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
+      <c r="E58" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
         <v>1</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>2</v>
       </c>
       <c r="C59">
         <v>15</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
+      <c r="E59" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
         <v>0.5</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>1.5</v>
       </c>
       <c r="C60">
         <v>15</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="2">
+      <c r="E60" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>2.5</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>2.25</v>
       </c>
       <c r="C61">
         <v>15</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="1">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="2">
+      <c r="E61" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
         <v>2.25</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>1.25</v>
       </c>
       <c r="C62">
         <v>15</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
+      <c r="E62" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
         <v>2.25</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>1.75</v>
       </c>
       <c r="C63">
         <v>15</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="1">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
+      <c r="E63" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
         <v>1.5</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>0.5</v>
       </c>
       <c r="C64">
         <v>15</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="1">
         <v>0.75</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0.09</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>